<commit_message>
update datamodel-code-generator to include the http extra; use figshare create private article metadata
</commit_message>
<xml_diff>
--- a/figleaf/figshare/researcher_metadata.xlsx
+++ b/figleaf/figshare/researcher_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scarlettv/figleaf/figleaf/figshare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6874670-728E-4E44-9541-DD7C1BCDFB9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D116AA-0CA5-A942-867D-1CFAB7FC6669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6260" yWindow="2780" windowWidth="28040" windowHeight="17440" xr2:uid="{F994D32C-DC09-7D4F-B37C-ED4B2EAE8784}"/>
   </bookViews>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
   <si>
     <t>Virginia Scarlett</t>
   </si>
   <si>
-    <t>Janelia Research Campus</t>
-  </si>
-  <si>
     <t>Attr_value</t>
   </si>
   <si>
@@ -56,21 +53,9 @@
     <t>Attr_key</t>
   </si>
   <si>
-    <t>publisher</t>
-  </si>
-  <si>
-    <t>publicationYear</t>
-  </si>
-  <si>
     <t>My cool dataset</t>
   </si>
   <si>
-    <t>nameType</t>
-  </si>
-  <si>
-    <t>Personal</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -80,39 +65,9 @@
     <t>William Shakespeare</t>
   </si>
   <si>
-    <t>nameIdentifiers</t>
-  </si>
-  <si>
-    <t>nameIdentifierScheme</t>
-  </si>
-  <si>
-    <t>schemeURI</t>
-  </si>
-  <si>
     <t>0000-0002-4156-2849</t>
   </si>
   <si>
-    <t>ORCID</t>
-  </si>
-  <si>
-    <t>https://orcid.org</t>
-  </si>
-  <si>
-    <t>University of California, Berkeley</t>
-  </si>
-  <si>
-    <t>HHMI Janelia Research Campus</t>
-  </si>
-  <si>
-    <t>titleType</t>
-  </si>
-  <si>
-    <t>Subtitle</t>
-  </si>
-  <si>
-    <t>An exploration of the meaning of life</t>
-  </si>
-  <si>
     <t>resourceType</t>
   </si>
   <si>
@@ -125,20 +80,47 @@
     <t>types</t>
   </si>
   <si>
-    <t>affiliations</t>
-  </si>
-  <si>
     <t>authors</t>
   </si>
   <si>
     <t>full_name</t>
+  </si>
+  <si>
+    <t>figshare_id</t>
+  </si>
+  <si>
+    <t>url_name</t>
+  </si>
+  <si>
+    <t>Virginia_Scarlett</t>
+  </si>
+  <si>
+    <t>orcid_id</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>While counting numbers is quite common, little is known about the true meaning of numbers. In this study, a series of random numbers was generated. Surprisingly, we found no evidence that numbers alone are inherently meaningful. This study suggests that numbers by themselves are not sufficient to explain their own meaning.</t>
+  </si>
+  <si>
+    <t>keywords</t>
+  </si>
+  <si>
+    <t>Single neuron reconstruction</t>
+  </si>
+  <si>
+    <t>categories</t>
+  </si>
+  <si>
+    <t>Neurosciences not elsewhere classified</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -167,6 +149,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -188,11 +176,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,37 +496,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F50D26F-5E03-AC45-84A4-9E66DD8565A6}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>0</v>
@@ -545,41 +534,41 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="D3" s="4">
+        <v>14526911</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>18</v>
@@ -587,149 +576,97 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="2">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="2">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="2">
-        <v>2</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="2">
-        <v>2</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>10</v>
+        <v>24</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="3">
-        <v>2023</v>
-      </c>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>